<commit_message>
GSYE-261: Implement tests for CommunityDatasheetParser
</commit_message>
<xml_diff>
--- a/tests/fixtures/community_datasheet.xlsx
+++ b/tests/fixtures/community_datasheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
   <si>
     <t>start_date</t>
   </si>
@@ -111,57 +111,6 @@
     <t>Carreg Winllan</t>
   </si>
   <si>
-    <t>Member 3</t>
-  </si>
-  <si>
-    <t>22 Palm Grove</t>
-  </si>
-  <si>
-    <t>Member 4</t>
-  </si>
-  <si>
-    <t>7 Broadway</t>
-  </si>
-  <si>
-    <t>Member 5</t>
-  </si>
-  <si>
-    <t>10 Pentaloe Close</t>
-  </si>
-  <si>
-    <t>Member 6</t>
-  </si>
-  <si>
-    <t>29 Lodge Avenue</t>
-  </si>
-  <si>
-    <t>Member 7</t>
-  </si>
-  <si>
-    <t>The Old Rectory</t>
-  </si>
-  <si>
-    <t>Member 8</t>
-  </si>
-  <si>
-    <t>26 Bosgate Close</t>
-  </si>
-  <si>
-    <t>Member 9</t>
-  </si>
-  <si>
-    <t>Starling Cottage</t>
-  </si>
-  <si>
-    <t>Member 10</t>
-  </si>
-  <si>
-    <t>Member 11</t>
-  </si>
-  <si>
-    <t>1 Butlers Cottages</t>
-  </si>
-  <si>
     <t>Member_name</t>
   </si>
   <si>
@@ -171,12 +120,6 @@
     <t>Load 1</t>
   </si>
   <si>
-    <t xml:space="preserve">Member 2 </t>
-  </si>
-  <si>
-    <t>Load 2</t>
-  </si>
-  <si>
     <t>PV_name</t>
   </si>
   <si>
@@ -192,9 +135,6 @@
     <t>PV 1</t>
   </si>
   <si>
-    <t>PV 2</t>
-  </si>
-  <si>
     <t>PV 3</t>
   </si>
   <si>
@@ -214,12 +154,6 @@
   </si>
   <si>
     <t>Battery 2</t>
-  </si>
-  <si>
-    <t>Battery 3</t>
-  </si>
-  <si>
-    <t>Battery 4</t>
   </si>
   <si>
     <t>Datetime</t>
@@ -322,13 +256,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1553,7 +1487,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1701,248 +1635,7 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" ht="15.35" customHeight="1">
-      <c r="A5" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="E5" s="6">
-        <v>1</v>
-      </c>
-      <c r="F5" s="6">
-        <v>7</v>
-      </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="7">
-        <v>0.12</v>
-      </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-    </row>
-    <row r="6" ht="15.35" customHeight="1">
-      <c r="A6" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="E6" s="6">
-        <v>1</v>
-      </c>
-      <c r="F6" s="6">
-        <v>7</v>
-      </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-    </row>
-    <row r="7" ht="15.35" customHeight="1">
-      <c r="A7" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="E7" s="6">
-        <v>1</v>
-      </c>
-      <c r="F7" s="6">
-        <v>7</v>
-      </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-    </row>
-    <row r="8" ht="15.35" customHeight="1">
-      <c r="A8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="E8" s="6">
-        <v>1</v>
-      </c>
-      <c r="F8" s="6">
-        <v>7</v>
-      </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-    </row>
-    <row r="9" ht="15.35" customHeight="1">
-      <c r="A9" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="E9" s="6">
-        <v>1</v>
-      </c>
-      <c r="F9" s="6">
-        <v>7</v>
-      </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-    </row>
-    <row r="10" ht="15.35" customHeight="1">
-      <c r="A10" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="E10" s="6">
-        <v>1</v>
-      </c>
-      <c r="F10" s="6">
-        <v>7</v>
-      </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-    </row>
-    <row r="11" ht="15.35" customHeight="1">
-      <c r="A11" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="E11" s="6">
-        <v>1</v>
-      </c>
-      <c r="F11" s="6">
-        <v>7</v>
-      </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-    </row>
-    <row r="12" ht="15.35" customHeight="1">
-      <c r="A12" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="6">
-        <v>1</v>
-      </c>
-      <c r="F12" s="6">
-        <v>7</v>
-      </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-    </row>
-    <row r="13" ht="15.35" customHeight="1">
-      <c r="A13" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="E13" s="6">
-        <v>1</v>
-      </c>
-      <c r="F13" s="6">
-        <v>7</v>
-      </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-    </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:P5">
-      <formula1>"Email,ZIP code,Location/Address (optional),Utility price,Feed-in Tariff,Grid fee,Taxes and surcharges,Fixed fee,Marketplace fee,Coefficient"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
@@ -1953,23 +1646,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="21.6719" style="8" customWidth="1"/>
-    <col min="2" max="5" width="10.8516" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="10.8516" style="8" customWidth="1"/>
+    <col min="1" max="1" width="21.6719" style="7" customWidth="1"/>
+    <col min="2" max="5" width="10.8516" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="10.8516" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.35" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -1980,19 +1673,15 @@
         <v>27</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="15.35" customHeight="1">
-      <c r="A3" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="B3" t="s" s="2">
-        <v>52</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -2033,18 +1722,11 @@
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="15.35" customHeight="1">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-    </row>
-    <row r="10" ht="15.35" customHeight="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2057,34 +1739,34 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="13.8516" style="9" customWidth="1"/>
-    <col min="2" max="2" width="10.8516" style="9" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="9" customWidth="1"/>
-    <col min="4" max="5" width="10.8516" style="9" customWidth="1"/>
-    <col min="6" max="16384" width="10.8516" style="9" customWidth="1"/>
+    <col min="1" max="1" width="13.8516" style="8" customWidth="1"/>
+    <col min="2" max="2" width="10.8516" style="8" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="8" customWidth="1"/>
+    <col min="4" max="5" width="10.8516" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="10.8516" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.35" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" ht="15.35" customHeight="1">
@@ -2092,41 +1774,37 @@
         <v>27</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="C2" s="4"/>
-      <c r="D2" s="7">
+      <c r="D2" s="9">
         <v>12</v>
       </c>
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="15.35" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="C3" s="6">
+        <v>12</v>
+      </c>
+      <c r="D3" s="9">
+        <v>32</v>
+      </c>
+      <c r="E3" s="6">
+        <v>123</v>
+      </c>
     </row>
     <row r="4" ht="15.35" customHeight="1">
-      <c r="A4" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="B4" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="C4" s="6">
-        <v>12</v>
-      </c>
-      <c r="D4" s="7">
-        <v>32</v>
-      </c>
-      <c r="E4" s="6">
-        <v>123</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" ht="15.35" customHeight="1">
       <c r="A5" s="2"/>
@@ -2157,18 +1835,11 @@
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="15.35" customHeight="1">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-    </row>
-    <row r="10" ht="15.35" customHeight="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2181,7 +1852,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2197,19 +1868,19 @@
   <sheetData>
     <row r="1" ht="15.35" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>63</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" ht="15.35" customHeight="1">
@@ -2217,7 +1888,7 @@
         <v>27</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2228,30 +1899,22 @@
         <v>29</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="15.35" customHeight="1">
-      <c r="A4" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="B4" t="s" s="2">
-        <v>66</v>
-      </c>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="15.35" customHeight="1">
-      <c r="A5" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="B5" t="s" s="2">
-        <v>67</v>
-      </c>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -2276,20 +1939,6 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-    </row>
-    <row r="9" ht="15.35" customHeight="1">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" ht="15.35" customHeight="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2302,100 +1951,70 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="19" style="11" customWidth="1"/>
-    <col min="2" max="5" width="10.8516" style="11" customWidth="1"/>
-    <col min="6" max="16384" width="10.8516" style="11" customWidth="1"/>
+    <col min="2" max="3" width="10.8516" style="11" customWidth="1"/>
+    <col min="4" max="16384" width="10.8516" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.35" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="D1" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="E1" t="s" s="2">
-        <v>58</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" ht="15.35" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="D2" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="E2" t="s" s="2">
-        <v>70</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" ht="15.35" customHeight="1">
       <c r="A3" s="12">
         <v>44410</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="9">
         <v>22.32</v>
       </c>
-      <c r="C3" s="7">
-        <v>16.91</v>
-      </c>
-      <c r="D3" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E3" s="7">
-        <v>2</v>
+      <c r="C3" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="4" ht="15.35" customHeight="1">
       <c r="A4" s="12">
         <v>44410.010416666664</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="9">
         <v>20.72</v>
       </c>
-      <c r="C4" s="7">
-        <v>17.17</v>
-      </c>
-      <c r="D4" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E4" s="7">
-        <v>2</v>
+      <c r="C4" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="5" ht="15.35" customHeight="1">
       <c r="A5" s="12">
         <v>44410.020833333336</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="9">
         <v>18.57</v>
       </c>
-      <c r="C5" s="7">
-        <v>17.17</v>
-      </c>
-      <c r="D5" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E5" s="7">
-        <v>3</v>
+      <c r="C5" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="6" ht="15.35" customHeight="1">
@@ -2403,1185 +2022,765 @@
         <v>44410.031249826388</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="7">
-        <v>17.42</v>
-      </c>
-      <c r="D6" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E6" s="7">
-        <v>6.09</v>
+      <c r="C6" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="7" ht="15.35" customHeight="1">
       <c r="A7" s="12">
         <v>44410.041666435187</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="9">
         <v>17.135</v>
       </c>
-      <c r="C7" s="7">
-        <v>17.55</v>
-      </c>
-      <c r="D7" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E7" s="7">
-        <v>4</v>
+      <c r="C7" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="8" ht="15.35" customHeight="1">
       <c r="A8" s="12">
         <v>44410.052083043978</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="9">
         <v>15.927</v>
       </c>
-      <c r="C8" s="7">
-        <v>17.703</v>
-      </c>
-      <c r="D8" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E8" s="7">
-        <v>5.845</v>
+      <c r="C8" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="9" ht="15.35" customHeight="1">
       <c r="A9" s="12">
         <v>44410.062499652777</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="9">
         <v>14.719</v>
       </c>
-      <c r="C9" s="7">
-        <v>17.856</v>
-      </c>
-      <c r="D9" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E9" s="7">
-        <v>6.654</v>
+      <c r="C9" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="10" ht="15.35" customHeight="1">
       <c r="A10" s="12">
         <v>44410.072916261575</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="9">
         <v>13.511</v>
       </c>
-      <c r="C10" s="7">
-        <v>18.009</v>
-      </c>
-      <c r="D10" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E10" s="7">
-        <v>7.463</v>
+      <c r="C10" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="11" ht="15.35" customHeight="1">
       <c r="A11" s="12">
         <v>44410.083332870374</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="9">
         <v>12.303</v>
       </c>
-      <c r="C11" s="7">
-        <v>18.162</v>
-      </c>
-      <c r="D11" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E11" s="7">
-        <v>8.272</v>
+      <c r="C11" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="12" ht="15.35" customHeight="1">
       <c r="A12" s="12">
         <v>44410.093749479165</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="9">
         <v>11.095</v>
       </c>
-      <c r="C12" s="7">
-        <v>18.315</v>
-      </c>
-      <c r="D12" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E12" s="7">
-        <v>9.081</v>
+      <c r="C12" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="13" ht="15.35" customHeight="1">
       <c r="A13" s="12">
         <v>44410.104166087964</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="9">
         <v>9.887</v>
       </c>
-      <c r="C13" s="7">
-        <v>18.468</v>
-      </c>
-      <c r="D13" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E13" s="7">
-        <v>9.890000000000001</v>
+      <c r="C13" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="14" ht="15.35" customHeight="1">
       <c r="A14" s="12">
         <v>44410.114582696762</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="9">
         <v>8.679</v>
       </c>
-      <c r="C14" s="7">
-        <v>18.621</v>
-      </c>
-      <c r="D14" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E14" s="7">
-        <v>10.699</v>
+      <c r="C14" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" s="12">
         <v>44410.124999305554</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="9">
         <v>7.471</v>
       </c>
-      <c r="C15" s="7">
-        <v>18.774</v>
-      </c>
-      <c r="D15" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E15" s="7">
-        <v>11.508</v>
+      <c r="C15" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="16" ht="15.35" customHeight="1">
       <c r="A16" s="12">
         <v>44410.135415914352</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="9">
         <v>6.263</v>
       </c>
-      <c r="C16" s="7">
-        <v>18.927</v>
-      </c>
-      <c r="D16" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E16" s="7">
-        <v>12.317</v>
+      <c r="C16" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" s="12">
         <v>44410.145832523151</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="9">
         <v>5.055</v>
       </c>
-      <c r="C17" s="7">
-        <v>19.08</v>
-      </c>
-      <c r="D17" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E17" s="7">
-        <v>13.126</v>
+      <c r="C17" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" s="12">
         <v>44410.156249131942</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="9">
         <v>3.847</v>
       </c>
-      <c r="C18" s="7">
-        <v>19.233</v>
-      </c>
-      <c r="D18" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E18" s="7">
-        <v>13.935</v>
+      <c r="C18" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="19" ht="15.35" customHeight="1">
       <c r="A19" s="12">
         <v>44410.166665740740</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="9">
         <v>2.639</v>
       </c>
-      <c r="C19" s="7">
-        <v>19.386</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="7">
-        <v>14.744</v>
-      </c>
+      <c r="C19" s="4"/>
     </row>
     <row r="20" ht="15.35" customHeight="1">
       <c r="A20" s="12">
         <v>44410.177082349539</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="9">
         <v>1.431</v>
       </c>
-      <c r="C20" s="7">
-        <v>19.539</v>
-      </c>
-      <c r="D20" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E20" s="7">
-        <v>15.553</v>
+      <c r="C20" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="21" ht="15.35" customHeight="1">
       <c r="A21" s="12">
         <v>44410.187498958330</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="9">
         <v>0.223000000000003</v>
       </c>
-      <c r="C21" s="7">
-        <v>19.692</v>
-      </c>
-      <c r="D21" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E21" s="7">
-        <v>16.362</v>
+      <c r="C21" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="22" ht="15.35" customHeight="1">
       <c r="A22" s="12">
         <v>44410.197915567129</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="9">
         <v>-0.984999999999999</v>
       </c>
-      <c r="C22" s="7">
-        <v>19.845</v>
-      </c>
-      <c r="D22" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E22" s="7">
-        <v>17.171</v>
+      <c r="C22" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="23" ht="15.35" customHeight="1">
       <c r="A23" s="12">
         <v>44410.208332175927</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="9">
         <v>-2.193</v>
       </c>
-      <c r="C23" s="7">
-        <v>19.998</v>
-      </c>
-      <c r="D23" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E23" s="7">
-        <v>17.98</v>
+      <c r="C23" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="24" ht="15.35" customHeight="1">
       <c r="A24" s="12">
         <v>44410.218748784719</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="9">
         <v>-3.401</v>
       </c>
-      <c r="C24" s="7">
-        <v>20.151</v>
-      </c>
-      <c r="D24" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E24" s="7">
-        <v>18.789</v>
+      <c r="C24" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="25" ht="15.35" customHeight="1">
       <c r="A25" s="12">
         <v>44410.229165393517</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="9">
         <v>-4.609</v>
       </c>
-      <c r="C25" s="7">
-        <v>20.304</v>
-      </c>
-      <c r="D25" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E25" s="7">
-        <v>19.598</v>
+      <c r="C25" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="26" ht="15.35" customHeight="1">
       <c r="A26" s="12">
         <v>44410.239582002316</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" s="9">
         <v>-5.817</v>
       </c>
-      <c r="C26" s="7">
-        <v>20.457</v>
-      </c>
-      <c r="D26" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E26" s="7">
-        <v>20.407</v>
+      <c r="C26" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="27" ht="15.35" customHeight="1">
       <c r="A27" s="12">
         <v>44410.249998611114</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="9">
         <v>-7.025</v>
       </c>
-      <c r="C27" s="7">
-        <v>20.61</v>
-      </c>
-      <c r="D27" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E27" s="7">
-        <v>21.216</v>
+      <c r="C27" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="28" ht="15.35" customHeight="1">
       <c r="A28" s="12">
         <v>44410.260415219906</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28" s="9">
         <v>-8.233000000000001</v>
       </c>
-      <c r="C28" s="7">
-        <v>20.763</v>
-      </c>
-      <c r="D28" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E28" s="7">
-        <v>22.025</v>
+      <c r="C28" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="29" ht="15.35" customHeight="1">
       <c r="A29" s="12">
         <v>44410.2708318287</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="9">
         <v>-9.441000000000001</v>
       </c>
-      <c r="C29" s="7">
-        <v>20.916</v>
-      </c>
-      <c r="D29" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E29" s="7">
-        <v>22.834</v>
+      <c r="C29" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="30" ht="15.35" customHeight="1">
       <c r="A30" s="12">
         <v>44410.2812484375</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" s="9">
         <v>-10.649</v>
       </c>
-      <c r="C30" s="7">
-        <v>21.069</v>
-      </c>
-      <c r="D30" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E30" s="7">
-        <v>23.643</v>
+      <c r="C30" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="31" ht="15.35" customHeight="1">
       <c r="A31" s="12">
         <v>44410.291665046294</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31" s="9">
         <v>-11.857</v>
       </c>
-      <c r="C31" s="7">
-        <v>21.222</v>
-      </c>
-      <c r="D31" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E31" s="7">
-        <v>24.452</v>
+      <c r="C31" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="32" ht="15.35" customHeight="1">
       <c r="A32" s="12">
         <v>44410.302081655092</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B32" s="9">
         <v>-13.065</v>
       </c>
-      <c r="C32" s="7">
-        <v>21.375</v>
-      </c>
-      <c r="D32" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E32" s="7">
-        <v>25.261</v>
+      <c r="C32" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="33" ht="15.35" customHeight="1">
       <c r="A33" s="12">
         <v>44410.312498263891</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B33" s="9">
         <v>-14.273</v>
       </c>
-      <c r="C33" s="7">
-        <v>21.528</v>
-      </c>
-      <c r="D33" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E33" s="7">
-        <v>26.07</v>
+      <c r="C33" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="34" ht="15.35" customHeight="1">
       <c r="A34" s="12">
         <v>44410.322914872682</v>
       </c>
-      <c r="B34" s="7">
+      <c r="B34" s="9">
         <v>-15.481</v>
       </c>
-      <c r="C34" s="7">
-        <v>21.681</v>
-      </c>
-      <c r="D34" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E34" s="7">
-        <v>26.879</v>
+      <c r="C34" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="35" ht="15.35" customHeight="1">
       <c r="A35" s="12">
         <v>44410.333331481481</v>
       </c>
-      <c r="B35" s="7">
+      <c r="B35" s="9">
         <v>-16.689</v>
       </c>
-      <c r="C35" s="7">
-        <v>21.834</v>
-      </c>
-      <c r="D35" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E35" s="7">
-        <v>27.688</v>
+      <c r="C35" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="36" ht="15.35" customHeight="1">
       <c r="A36" s="12">
         <v>44410.343748090279</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B36" s="9">
         <v>-17.897</v>
       </c>
-      <c r="C36" s="7">
-        <v>21.987</v>
-      </c>
-      <c r="D36" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E36" s="7">
-        <v>28.497</v>
+      <c r="C36" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="37" ht="15.35" customHeight="1">
       <c r="A37" s="12">
         <v>44410.354164699071</v>
       </c>
-      <c r="B37" s="7">
+      <c r="B37" s="9">
         <v>-19.105</v>
       </c>
-      <c r="C37" s="7">
-        <v>22.14</v>
-      </c>
-      <c r="D37" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E37" s="7">
-        <v>29.306</v>
+      <c r="C37" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="38" ht="15.35" customHeight="1">
       <c r="A38" s="12">
         <v>44410.364581307869</v>
       </c>
-      <c r="B38" s="7">
+      <c r="B38" s="9">
         <v>-20.313</v>
       </c>
-      <c r="C38" s="7">
-        <v>22.293</v>
-      </c>
-      <c r="D38" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E38" s="7">
-        <v>30.115</v>
+      <c r="C38" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="39" ht="15.35" customHeight="1">
       <c r="A39" s="12">
         <v>44410.374997916668</v>
       </c>
-      <c r="B39" s="7">
+      <c r="B39" s="9">
         <v>-21.521</v>
       </c>
-      <c r="C39" s="7">
-        <v>22.446</v>
-      </c>
-      <c r="D39" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E39" s="7">
-        <v>30.924</v>
+      <c r="C39" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="40" ht="15.35" customHeight="1">
       <c r="A40" s="12">
         <v>44410.385414525466</v>
       </c>
-      <c r="B40" s="7">
+      <c r="B40" s="9">
         <v>-22.729</v>
       </c>
-      <c r="C40" s="7">
-        <v>22.599</v>
-      </c>
-      <c r="D40" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E40" s="7">
-        <v>31.733</v>
+      <c r="C40" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="41" ht="15.35" customHeight="1">
       <c r="A41" s="12">
         <v>44410.395831134258</v>
       </c>
-      <c r="B41" s="7">
+      <c r="B41" s="9">
         <v>-23.937</v>
       </c>
-      <c r="C41" s="7">
-        <v>22.752</v>
-      </c>
-      <c r="D41" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E41" s="7">
-        <v>32.542</v>
+      <c r="C41" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="42" ht="15.35" customHeight="1">
       <c r="A42" s="12">
         <v>44410.406247743056</v>
       </c>
-      <c r="B42" s="7">
+      <c r="B42" s="9">
         <v>-25.145</v>
       </c>
-      <c r="C42" s="7">
-        <v>22.905</v>
-      </c>
-      <c r="D42" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E42" s="7">
-        <v>33.351</v>
+      <c r="C42" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="43" ht="15.35" customHeight="1">
       <c r="A43" s="12">
         <v>44410.416664351855</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B43" s="9">
         <v>-26.353</v>
       </c>
-      <c r="C43" s="7">
-        <v>23.058</v>
-      </c>
-      <c r="D43" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E43" s="7">
-        <v>34.16</v>
+      <c r="C43" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="44" ht="15.35" customHeight="1">
       <c r="A44" s="12">
         <v>44410.427080960646</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B44" s="9">
         <v>-27.561</v>
       </c>
-      <c r="C44" s="7">
-        <v>23.211</v>
-      </c>
-      <c r="D44" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E44" s="7">
-        <v>34.969</v>
+      <c r="C44" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="45" ht="15.35" customHeight="1">
       <c r="A45" s="12">
         <v>44410.437497569445</v>
       </c>
-      <c r="B45" s="7">
+      <c r="B45" s="9">
         <v>-28.769</v>
       </c>
-      <c r="C45" s="7">
-        <v>23.364</v>
-      </c>
-      <c r="D45" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E45" s="7">
-        <v>35.778</v>
+      <c r="C45" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="46" ht="15.35" customHeight="1">
       <c r="A46" s="12">
         <v>44410.447914178243</v>
       </c>
-      <c r="B46" s="7">
+      <c r="B46" s="9">
         <v>-29.977</v>
       </c>
-      <c r="C46" s="7">
-        <v>23.517</v>
-      </c>
-      <c r="D46" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E46" s="7">
-        <v>36.587</v>
+      <c r="C46" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="47" ht="15.35" customHeight="1">
       <c r="A47" s="12">
         <v>44410.458330787034</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B47" s="9">
         <v>-31.185</v>
       </c>
-      <c r="C47" s="7">
-        <v>23.67</v>
-      </c>
-      <c r="D47" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E47" s="7">
-        <v>37.396</v>
+      <c r="C47" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="48" ht="15.35" customHeight="1">
       <c r="A48" s="12">
         <v>44410.468747395833</v>
       </c>
-      <c r="B48" s="7">
+      <c r="B48" s="9">
         <v>-32.393</v>
       </c>
-      <c r="C48" s="7">
-        <v>23.823</v>
-      </c>
-      <c r="D48" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E48" s="7">
-        <v>38.205</v>
+      <c r="C48" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="49" ht="15.35" customHeight="1">
       <c r="A49" s="12">
         <v>44410.479164004631</v>
       </c>
-      <c r="B49" s="7">
+      <c r="B49" s="9">
         <v>-33.601</v>
       </c>
-      <c r="C49" s="7">
-        <v>23.976</v>
-      </c>
-      <c r="D49" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E49" s="7">
-        <v>39.014</v>
+      <c r="C49" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="50" ht="15.35" customHeight="1">
       <c r="A50" s="12">
         <v>44410.489580613423</v>
       </c>
-      <c r="B50" s="7">
+      <c r="B50" s="9">
         <v>-34.809</v>
       </c>
-      <c r="C50" s="7">
-        <v>24.129</v>
-      </c>
-      <c r="D50" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E50" s="7">
-        <v>39.823</v>
+      <c r="C50" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="51" ht="15.35" customHeight="1">
       <c r="A51" s="12">
         <v>44410.499997222221</v>
       </c>
-      <c r="B51" s="7">
+      <c r="B51" s="9">
         <v>-36.017</v>
       </c>
-      <c r="C51" s="7">
-        <v>24.282</v>
-      </c>
-      <c r="D51" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E51" s="7">
-        <v>40.632</v>
+      <c r="C51" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="52" ht="15.35" customHeight="1">
       <c r="A52" s="12">
         <v>44410.510413831020</v>
       </c>
-      <c r="B52" s="7">
+      <c r="B52" s="9">
         <v>-37.225</v>
       </c>
-      <c r="C52" s="7">
-        <v>24.435</v>
-      </c>
-      <c r="D52" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E52" s="7">
-        <v>41.441</v>
+      <c r="C52" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="53" ht="15.35" customHeight="1">
       <c r="A53" s="12">
         <v>44410.520830439818</v>
       </c>
-      <c r="B53" s="7">
+      <c r="B53" s="9">
         <v>-38.433</v>
       </c>
-      <c r="C53" s="7">
-        <v>24.588</v>
-      </c>
-      <c r="D53" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E53" s="7">
-        <v>42.25</v>
+      <c r="C53" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="54" ht="15.35" customHeight="1">
       <c r="A54" s="12">
         <v>44410.531247048610</v>
       </c>
-      <c r="B54" s="7">
+      <c r="B54" s="9">
         <v>-39.641</v>
       </c>
-      <c r="C54" s="7">
-        <v>24.741</v>
-      </c>
-      <c r="D54" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E54" s="7">
-        <v>43.059</v>
+      <c r="C54" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="55" ht="15.35" customHeight="1">
       <c r="A55" s="12">
         <v>44410.541663657408</v>
       </c>
-      <c r="B55" s="7">
+      <c r="B55" s="9">
         <v>-40.849</v>
       </c>
-      <c r="C55" s="7">
-        <v>24.894</v>
-      </c>
-      <c r="D55" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E55" s="7">
-        <v>43.868</v>
+      <c r="C55" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="56" ht="15.35" customHeight="1">
       <c r="A56" s="12">
         <v>44410.552080266207</v>
       </c>
-      <c r="B56" s="7">
+      <c r="B56" s="9">
         <v>-42.057</v>
       </c>
-      <c r="C56" s="7">
-        <v>25.047</v>
-      </c>
-      <c r="D56" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E56" s="7">
-        <v>44.677</v>
+      <c r="C56" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="57" ht="15.35" customHeight="1">
       <c r="A57" s="12">
         <v>44410.562496875</v>
       </c>
-      <c r="B57" s="7">
+      <c r="B57" s="9">
         <v>-43.265</v>
       </c>
-      <c r="C57" s="7">
-        <v>25.2</v>
-      </c>
-      <c r="D57" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E57" s="7">
-        <v>45.486</v>
+      <c r="C57" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="58" ht="15.35" customHeight="1">
       <c r="A58" s="12">
         <v>44410.5729134838</v>
       </c>
-      <c r="B58" s="7">
+      <c r="B58" s="9">
         <v>-44.473</v>
       </c>
-      <c r="C58" s="7">
-        <v>25.353</v>
-      </c>
-      <c r="D58" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E58" s="7">
-        <v>46.295</v>
+      <c r="C58" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="59" ht="15.35" customHeight="1">
       <c r="A59" s="12">
         <v>44410.5833300926</v>
       </c>
-      <c r="B59" s="7">
+      <c r="B59" s="9">
         <v>-45.681</v>
       </c>
-      <c r="C59" s="7">
-        <v>25.506</v>
-      </c>
-      <c r="D59" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E59" s="7">
-        <v>47.104</v>
+      <c r="C59" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="60" ht="15.35" customHeight="1">
       <c r="A60" s="12">
         <v>44410.593746701386</v>
       </c>
-      <c r="B60" s="7">
+      <c r="B60" s="9">
         <v>-46.889</v>
       </c>
-      <c r="C60" s="7">
-        <v>25.659</v>
-      </c>
-      <c r="D60" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E60" s="7">
-        <v>47.913</v>
+      <c r="C60" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="61" ht="15.35" customHeight="1">
       <c r="A61" s="12">
         <v>44410.604163310185</v>
       </c>
-      <c r="B61" s="7">
+      <c r="B61" s="9">
         <v>-48.097</v>
       </c>
-      <c r="C61" s="7">
-        <v>25.812</v>
-      </c>
-      <c r="D61" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E61" s="7">
-        <v>48.722</v>
+      <c r="C61" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="62" ht="15.35" customHeight="1">
       <c r="A62" s="12">
         <v>44410.614579918984</v>
       </c>
-      <c r="B62" s="7">
+      <c r="B62" s="9">
         <v>-49.305</v>
       </c>
-      <c r="C62" s="7">
-        <v>25.965</v>
-      </c>
-      <c r="D62" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E62" s="7">
-        <v>49.531</v>
+      <c r="C62" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="63" ht="15.35" customHeight="1">
       <c r="A63" s="12">
         <v>44410.624996527775</v>
       </c>
-      <c r="B63" s="7">
+      <c r="B63" s="9">
         <v>-50.513</v>
       </c>
-      <c r="C63" s="7">
-        <v>26.118</v>
-      </c>
-      <c r="D63" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E63" s="7">
-        <v>50.34</v>
+      <c r="C63" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="64" ht="15.35" customHeight="1">
       <c r="A64" s="12">
         <v>44410.635413136573</v>
       </c>
-      <c r="B64" s="7">
+      <c r="B64" s="9">
         <v>-51.721</v>
       </c>
-      <c r="C64" s="7">
-        <v>26.271</v>
-      </c>
-      <c r="D64" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E64" s="7">
-        <v>51.149</v>
+      <c r="C64" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="65" ht="15.35" customHeight="1">
       <c r="A65" s="12">
         <v>44410.645829745372</v>
       </c>
-      <c r="B65" s="7">
+      <c r="B65" s="9">
         <v>-52.929</v>
       </c>
-      <c r="C65" s="7">
-        <v>26.424</v>
-      </c>
-      <c r="D65" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E65" s="7">
-        <v>51.958</v>
+      <c r="C65" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="66" ht="15.35" customHeight="1">
       <c r="A66" s="12">
         <v>44410.656246354163</v>
       </c>
-      <c r="B66" s="7">
+      <c r="B66" s="9">
         <v>-54.137</v>
       </c>
-      <c r="C66" s="7">
-        <v>26.577</v>
-      </c>
-      <c r="D66" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E66" s="7">
-        <v>52.767</v>
+      <c r="C66" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="67" ht="15.35" customHeight="1">
       <c r="A67" s="12">
         <v>44410.666662962962</v>
       </c>
-      <c r="B67" s="7">
+      <c r="B67" s="9">
         <v>-55.345</v>
       </c>
-      <c r="C67" s="7">
-        <v>26.73</v>
-      </c>
-      <c r="D67" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E67" s="7">
-        <v>53.576</v>
+      <c r="C67" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="68" ht="15.35" customHeight="1">
       <c r="A68" s="12">
         <v>44410.677079571760</v>
       </c>
-      <c r="B68" s="7">
+      <c r="B68" s="9">
         <v>-56.553</v>
       </c>
-      <c r="C68" s="7">
-        <v>26.883</v>
-      </c>
-      <c r="D68" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E68" s="7">
-        <v>54.385</v>
+      <c r="C68" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="69" ht="15.35" customHeight="1">
       <c r="A69" s="12">
         <v>44410.687496180559</v>
       </c>
-      <c r="B69" s="7">
+      <c r="B69" s="9">
         <v>-57.761</v>
       </c>
-      <c r="C69" s="7">
-        <v>27.036</v>
-      </c>
-      <c r="D69" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E69" s="7">
-        <v>55.194</v>
+      <c r="C69" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="70" ht="15.35" customHeight="1">
       <c r="A70" s="12">
         <v>44410.697912789350</v>
       </c>
-      <c r="B70" s="7">
+      <c r="B70" s="9">
         <v>-58.969</v>
       </c>
-      <c r="C70" s="7">
-        <v>27.189</v>
-      </c>
-      <c r="D70" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E70" s="7">
-        <v>56.003</v>
+      <c r="C70" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="71" ht="15.35" customHeight="1">
       <c r="A71" s="12">
         <v>44410.708329398149</v>
       </c>
-      <c r="B71" s="7">
+      <c r="B71" s="9">
         <v>-60.177</v>
       </c>
-      <c r="C71" s="7">
-        <v>27.342</v>
-      </c>
-      <c r="D71" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E71" s="7">
-        <v>56.812</v>
+      <c r="C71" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="72" ht="15.35" customHeight="1">
       <c r="A72" s="12">
         <v>44410.718746006947</v>
       </c>
-      <c r="B72" s="7">
+      <c r="B72" s="9">
         <v>-61.385</v>
       </c>
-      <c r="C72" s="7">
-        <v>27.495</v>
-      </c>
-      <c r="D72" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E72" s="7">
-        <v>57.621</v>
+      <c r="C72" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="73" ht="15.35" customHeight="1">
       <c r="A73" s="12">
         <v>44410.729162615738</v>
       </c>
-      <c r="B73" s="7">
+      <c r="B73" s="9">
         <v>-62.593</v>
       </c>
-      <c r="C73" s="7">
-        <v>27.648</v>
-      </c>
-      <c r="D73" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E73" s="7">
-        <v>58.43</v>
+      <c r="C73" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="74" ht="15.35" customHeight="1">
       <c r="A74" s="12">
         <v>44410.739579224537</v>
       </c>
-      <c r="B74" s="7">
+      <c r="B74" s="9">
         <v>-63.801</v>
       </c>
-      <c r="C74" s="7">
-        <v>27.801</v>
-      </c>
-      <c r="D74" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E74" s="7">
-        <v>59.239</v>
+      <c r="C74" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="75" ht="15.35" customHeight="1">
       <c r="A75" s="12">
         <v>44410.749995833336</v>
       </c>
-      <c r="B75" s="7">
+      <c r="B75" s="9">
         <v>-65.009</v>
       </c>
-      <c r="C75" s="7">
-        <v>27.954</v>
-      </c>
-      <c r="D75" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E75" s="7">
-        <v>60.048</v>
+      <c r="C75" s="9">
+        <v>11.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GSYE-261: Update community datasheet tests file
This fixes some validation issues
</commit_message>
<xml_diff>
--- a/tests/fixtures/community_datasheet.xlsx
+++ b/tests/fixtures/community_datasheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
   <si>
     <t>start_date</t>
   </si>
@@ -102,13 +102,27 @@
     <t>Member 1</t>
   </si>
   <si>
-    <t>10210 La Loge-Pomblin, France</t>
+    <t>some-email-1@some-email.com</t>
+  </si>
+  <si>
+    <t>Am Werth 94, Wolffburg, Schleswig-Holstein, Germany</t>
   </si>
   <si>
     <t>Member 2</t>
   </si>
   <si>
-    <t>Carreg Winllan</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>some-email-2@some-email.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Heisterbachstr. 8, Ost Colin, Hamburg, Germany</t>
   </si>
   <si>
     <t>Member_name</t>
@@ -174,7 +188,7 @@
     <numFmt numFmtId="59" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
     <numFmt numFmtId="60" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd&quot; &quot;hh:mm"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -188,6 +202,12 @@
     <font>
       <sz val="15"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="12"/>
+      <color indexed="11"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -293,6 +313,7 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1494,7 +1515,8 @@
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="16" style="5" customWidth="1"/>
-    <col min="2" max="3" width="10.8516" style="5" customWidth="1"/>
+    <col min="2" max="2" width="27.3516" style="5" customWidth="1"/>
+    <col min="3" max="3" width="10.8516" style="5" customWidth="1"/>
     <col min="4" max="4" width="24.3516" style="5" customWidth="1"/>
     <col min="5" max="10" width="21.6719" style="5" customWidth="1"/>
     <col min="11" max="11" width="10.8516" style="5" customWidth="1"/>
@@ -1587,10 +1609,14 @@
       <c r="A3" t="s" s="2">
         <v>27</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="B3" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="C3" s="6">
+        <v>64508</v>
+      </c>
       <c r="D3" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E3" s="6">
         <v>1</v>
@@ -1598,11 +1624,21 @@
       <c r="F3" s="6">
         <v>7</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
+      <c r="G3" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0.5</v>
+      </c>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
@@ -1611,12 +1647,16 @@
     </row>
     <row r="4" ht="15.35" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>29</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="C4" s="6">
+        <v>57441</v>
+      </c>
       <c r="D4" t="s" s="2">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E4" s="6">
         <v>1</v>
@@ -1624,11 +1664,21 @@
       <c r="F4" s="6">
         <v>7</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
+      <c r="G4" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0.5</v>
+      </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
@@ -1636,6 +1686,9 @@
       <c r="P4" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" location="" tooltip="" display="some-email-2@some-email.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
@@ -1659,10 +1712,10 @@
   <sheetData>
     <row r="1" ht="15.35" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -1673,7 +1726,7 @@
         <v>27</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -1754,19 +1807,19 @@
   <sheetData>
     <row r="1" ht="15.35" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" ht="15.35" customHeight="1">
@@ -1774,7 +1827,7 @@
         <v>27</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="9">
@@ -1784,10 +1837,10 @@
     </row>
     <row r="3" ht="15.35" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C3" s="6">
         <v>12</v>
@@ -1868,19 +1921,19 @@
   <sheetData>
     <row r="1" ht="15.35" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" ht="15.35" customHeight="1">
@@ -1888,22 +1941,34 @@
         <v>27</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+        <v>46</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="D2" s="6">
+        <v>10</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="3" ht="15.35" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="6">
+        <v>13</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="4" ht="15.35" customHeight="1">
       <c r="A4" s="4"/>
@@ -1964,24 +2029,24 @@
   <sheetData>
     <row r="1" ht="15.35" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" ht="15.35" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" ht="15.35" customHeight="1">

</xml_diff>

<commit_message>
GSYE-261: Shorten profiles in datasheet test excel file
</commit_message>
<xml_diff>
--- a/tests/fixtures/community_datasheet.xlsx
+++ b/tests/fixtures/community_datasheet.xlsx
@@ -2016,7 +2016,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2062,7 +2062,7 @@
     </row>
     <row r="4" ht="15.35" customHeight="1">
       <c r="A4" s="12">
-        <v>44410.010416666664</v>
+        <v>44410.041666666664</v>
       </c>
       <c r="B4" s="9">
         <v>20.72</v>
@@ -2073,7 +2073,7 @@
     </row>
     <row r="5" ht="15.35" customHeight="1">
       <c r="A5" s="12">
-        <v>44410.020833333336</v>
+        <v>44410.083333333336</v>
       </c>
       <c r="B5" s="9">
         <v>18.57</v>
@@ -2084,7 +2084,7 @@
     </row>
     <row r="6" ht="15.35" customHeight="1">
       <c r="A6" s="12">
-        <v>44410.031249826388</v>
+        <v>44410.125</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="9">
@@ -2093,7 +2093,7 @@
     </row>
     <row r="7" ht="15.35" customHeight="1">
       <c r="A7" s="12">
-        <v>44410.041666435187</v>
+        <v>44410.166666666664</v>
       </c>
       <c r="B7" s="9">
         <v>17.135</v>
@@ -2104,7 +2104,7 @@
     </row>
     <row r="8" ht="15.35" customHeight="1">
       <c r="A8" s="12">
-        <v>44410.052083043978</v>
+        <v>44410.208333333336</v>
       </c>
       <c r="B8" s="9">
         <v>15.927</v>
@@ -2115,7 +2115,7 @@
     </row>
     <row r="9" ht="15.35" customHeight="1">
       <c r="A9" s="12">
-        <v>44410.062499652777</v>
+        <v>44410.25</v>
       </c>
       <c r="B9" s="9">
         <v>14.719</v>
@@ -2126,7 +2126,7 @@
     </row>
     <row r="10" ht="15.35" customHeight="1">
       <c r="A10" s="12">
-        <v>44410.072916261575</v>
+        <v>44410.291666666664</v>
       </c>
       <c r="B10" s="9">
         <v>13.511</v>
@@ -2137,7 +2137,7 @@
     </row>
     <row r="11" ht="15.35" customHeight="1">
       <c r="A11" s="12">
-        <v>44410.083332870374</v>
+        <v>44410.333333333336</v>
       </c>
       <c r="B11" s="9">
         <v>12.303</v>
@@ -2148,7 +2148,7 @@
     </row>
     <row r="12" ht="15.35" customHeight="1">
       <c r="A12" s="12">
-        <v>44410.093749479165</v>
+        <v>44410.375</v>
       </c>
       <c r="B12" s="9">
         <v>11.095</v>
@@ -2159,7 +2159,7 @@
     </row>
     <row r="13" ht="15.35" customHeight="1">
       <c r="A13" s="12">
-        <v>44410.104166087964</v>
+        <v>44410.416666666664</v>
       </c>
       <c r="B13" s="9">
         <v>9.887</v>
@@ -2170,7 +2170,7 @@
     </row>
     <row r="14" ht="15.35" customHeight="1">
       <c r="A14" s="12">
-        <v>44410.114582696762</v>
+        <v>44410.458333333336</v>
       </c>
       <c r="B14" s="9">
         <v>8.679</v>
@@ -2181,7 +2181,7 @@
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" s="12">
-        <v>44410.124999305554</v>
+        <v>44410.5</v>
       </c>
       <c r="B15" s="9">
         <v>7.471</v>
@@ -2192,7 +2192,7 @@
     </row>
     <row r="16" ht="15.35" customHeight="1">
       <c r="A16" s="12">
-        <v>44410.135415914352</v>
+        <v>44410.541666666664</v>
       </c>
       <c r="B16" s="9">
         <v>6.263</v>
@@ -2203,7 +2203,7 @@
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" s="12">
-        <v>44410.145832523151</v>
+        <v>44410.583333333336</v>
       </c>
       <c r="B17" s="9">
         <v>5.055</v>
@@ -2214,7 +2214,7 @@
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" s="12">
-        <v>44410.156249131942</v>
+        <v>44410.625</v>
       </c>
       <c r="B18" s="9">
         <v>3.847</v>
@@ -2225,628 +2225,12 @@
     </row>
     <row r="19" ht="15.35" customHeight="1">
       <c r="A19" s="12">
-        <v>44410.166665740740</v>
+        <v>44410.666666666664</v>
       </c>
       <c r="B19" s="9">
         <v>2.639</v>
       </c>
       <c r="C19" s="4"/>
-    </row>
-    <row r="20" ht="15.35" customHeight="1">
-      <c r="A20" s="12">
-        <v>44410.177082349539</v>
-      </c>
-      <c r="B20" s="9">
-        <v>1.431</v>
-      </c>
-      <c r="C20" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="21" ht="15.35" customHeight="1">
-      <c r="A21" s="12">
-        <v>44410.187498958330</v>
-      </c>
-      <c r="B21" s="9">
-        <v>0.223000000000003</v>
-      </c>
-      <c r="C21" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="22" ht="15.35" customHeight="1">
-      <c r="A22" s="12">
-        <v>44410.197915567129</v>
-      </c>
-      <c r="B22" s="9">
-        <v>-0.984999999999999</v>
-      </c>
-      <c r="C22" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="23" ht="15.35" customHeight="1">
-      <c r="A23" s="12">
-        <v>44410.208332175927</v>
-      </c>
-      <c r="B23" s="9">
-        <v>-2.193</v>
-      </c>
-      <c r="C23" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="24" ht="15.35" customHeight="1">
-      <c r="A24" s="12">
-        <v>44410.218748784719</v>
-      </c>
-      <c r="B24" s="9">
-        <v>-3.401</v>
-      </c>
-      <c r="C24" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="25" ht="15.35" customHeight="1">
-      <c r="A25" s="12">
-        <v>44410.229165393517</v>
-      </c>
-      <c r="B25" s="9">
-        <v>-4.609</v>
-      </c>
-      <c r="C25" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="26" ht="15.35" customHeight="1">
-      <c r="A26" s="12">
-        <v>44410.239582002316</v>
-      </c>
-      <c r="B26" s="9">
-        <v>-5.817</v>
-      </c>
-      <c r="C26" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="27" ht="15.35" customHeight="1">
-      <c r="A27" s="12">
-        <v>44410.249998611114</v>
-      </c>
-      <c r="B27" s="9">
-        <v>-7.025</v>
-      </c>
-      <c r="C27" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="28" ht="15.35" customHeight="1">
-      <c r="A28" s="12">
-        <v>44410.260415219906</v>
-      </c>
-      <c r="B28" s="9">
-        <v>-8.233000000000001</v>
-      </c>
-      <c r="C28" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="29" ht="15.35" customHeight="1">
-      <c r="A29" s="12">
-        <v>44410.2708318287</v>
-      </c>
-      <c r="B29" s="9">
-        <v>-9.441000000000001</v>
-      </c>
-      <c r="C29" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="30" ht="15.35" customHeight="1">
-      <c r="A30" s="12">
-        <v>44410.2812484375</v>
-      </c>
-      <c r="B30" s="9">
-        <v>-10.649</v>
-      </c>
-      <c r="C30" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="31" ht="15.35" customHeight="1">
-      <c r="A31" s="12">
-        <v>44410.291665046294</v>
-      </c>
-      <c r="B31" s="9">
-        <v>-11.857</v>
-      </c>
-      <c r="C31" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="32" ht="15.35" customHeight="1">
-      <c r="A32" s="12">
-        <v>44410.302081655092</v>
-      </c>
-      <c r="B32" s="9">
-        <v>-13.065</v>
-      </c>
-      <c r="C32" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="33" ht="15.35" customHeight="1">
-      <c r="A33" s="12">
-        <v>44410.312498263891</v>
-      </c>
-      <c r="B33" s="9">
-        <v>-14.273</v>
-      </c>
-      <c r="C33" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="34" ht="15.35" customHeight="1">
-      <c r="A34" s="12">
-        <v>44410.322914872682</v>
-      </c>
-      <c r="B34" s="9">
-        <v>-15.481</v>
-      </c>
-      <c r="C34" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="35" ht="15.35" customHeight="1">
-      <c r="A35" s="12">
-        <v>44410.333331481481</v>
-      </c>
-      <c r="B35" s="9">
-        <v>-16.689</v>
-      </c>
-      <c r="C35" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="36" ht="15.35" customHeight="1">
-      <c r="A36" s="12">
-        <v>44410.343748090279</v>
-      </c>
-      <c r="B36" s="9">
-        <v>-17.897</v>
-      </c>
-      <c r="C36" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="37" ht="15.35" customHeight="1">
-      <c r="A37" s="12">
-        <v>44410.354164699071</v>
-      </c>
-      <c r="B37" s="9">
-        <v>-19.105</v>
-      </c>
-      <c r="C37" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="38" ht="15.35" customHeight="1">
-      <c r="A38" s="12">
-        <v>44410.364581307869</v>
-      </c>
-      <c r="B38" s="9">
-        <v>-20.313</v>
-      </c>
-      <c r="C38" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="39" ht="15.35" customHeight="1">
-      <c r="A39" s="12">
-        <v>44410.374997916668</v>
-      </c>
-      <c r="B39" s="9">
-        <v>-21.521</v>
-      </c>
-      <c r="C39" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="40" ht="15.35" customHeight="1">
-      <c r="A40" s="12">
-        <v>44410.385414525466</v>
-      </c>
-      <c r="B40" s="9">
-        <v>-22.729</v>
-      </c>
-      <c r="C40" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="41" ht="15.35" customHeight="1">
-      <c r="A41" s="12">
-        <v>44410.395831134258</v>
-      </c>
-      <c r="B41" s="9">
-        <v>-23.937</v>
-      </c>
-      <c r="C41" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="42" ht="15.35" customHeight="1">
-      <c r="A42" s="12">
-        <v>44410.406247743056</v>
-      </c>
-      <c r="B42" s="9">
-        <v>-25.145</v>
-      </c>
-      <c r="C42" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="43" ht="15.35" customHeight="1">
-      <c r="A43" s="12">
-        <v>44410.416664351855</v>
-      </c>
-      <c r="B43" s="9">
-        <v>-26.353</v>
-      </c>
-      <c r="C43" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="44" ht="15.35" customHeight="1">
-      <c r="A44" s="12">
-        <v>44410.427080960646</v>
-      </c>
-      <c r="B44" s="9">
-        <v>-27.561</v>
-      </c>
-      <c r="C44" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="45" ht="15.35" customHeight="1">
-      <c r="A45" s="12">
-        <v>44410.437497569445</v>
-      </c>
-      <c r="B45" s="9">
-        <v>-28.769</v>
-      </c>
-      <c r="C45" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="46" ht="15.35" customHeight="1">
-      <c r="A46" s="12">
-        <v>44410.447914178243</v>
-      </c>
-      <c r="B46" s="9">
-        <v>-29.977</v>
-      </c>
-      <c r="C46" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="47" ht="15.35" customHeight="1">
-      <c r="A47" s="12">
-        <v>44410.458330787034</v>
-      </c>
-      <c r="B47" s="9">
-        <v>-31.185</v>
-      </c>
-      <c r="C47" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="48" ht="15.35" customHeight="1">
-      <c r="A48" s="12">
-        <v>44410.468747395833</v>
-      </c>
-      <c r="B48" s="9">
-        <v>-32.393</v>
-      </c>
-      <c r="C48" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="49" ht="15.35" customHeight="1">
-      <c r="A49" s="12">
-        <v>44410.479164004631</v>
-      </c>
-      <c r="B49" s="9">
-        <v>-33.601</v>
-      </c>
-      <c r="C49" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="50" ht="15.35" customHeight="1">
-      <c r="A50" s="12">
-        <v>44410.489580613423</v>
-      </c>
-      <c r="B50" s="9">
-        <v>-34.809</v>
-      </c>
-      <c r="C50" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="51" ht="15.35" customHeight="1">
-      <c r="A51" s="12">
-        <v>44410.499997222221</v>
-      </c>
-      <c r="B51" s="9">
-        <v>-36.017</v>
-      </c>
-      <c r="C51" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="52" ht="15.35" customHeight="1">
-      <c r="A52" s="12">
-        <v>44410.510413831020</v>
-      </c>
-      <c r="B52" s="9">
-        <v>-37.225</v>
-      </c>
-      <c r="C52" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="53" ht="15.35" customHeight="1">
-      <c r="A53" s="12">
-        <v>44410.520830439818</v>
-      </c>
-      <c r="B53" s="9">
-        <v>-38.433</v>
-      </c>
-      <c r="C53" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="54" ht="15.35" customHeight="1">
-      <c r="A54" s="12">
-        <v>44410.531247048610</v>
-      </c>
-      <c r="B54" s="9">
-        <v>-39.641</v>
-      </c>
-      <c r="C54" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="55" ht="15.35" customHeight="1">
-      <c r="A55" s="12">
-        <v>44410.541663657408</v>
-      </c>
-      <c r="B55" s="9">
-        <v>-40.849</v>
-      </c>
-      <c r="C55" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="56" ht="15.35" customHeight="1">
-      <c r="A56" s="12">
-        <v>44410.552080266207</v>
-      </c>
-      <c r="B56" s="9">
-        <v>-42.057</v>
-      </c>
-      <c r="C56" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="57" ht="15.35" customHeight="1">
-      <c r="A57" s="12">
-        <v>44410.562496875</v>
-      </c>
-      <c r="B57" s="9">
-        <v>-43.265</v>
-      </c>
-      <c r="C57" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="58" ht="15.35" customHeight="1">
-      <c r="A58" s="12">
-        <v>44410.5729134838</v>
-      </c>
-      <c r="B58" s="9">
-        <v>-44.473</v>
-      </c>
-      <c r="C58" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="59" ht="15.35" customHeight="1">
-      <c r="A59" s="12">
-        <v>44410.5833300926</v>
-      </c>
-      <c r="B59" s="9">
-        <v>-45.681</v>
-      </c>
-      <c r="C59" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="60" ht="15.35" customHeight="1">
-      <c r="A60" s="12">
-        <v>44410.593746701386</v>
-      </c>
-      <c r="B60" s="9">
-        <v>-46.889</v>
-      </c>
-      <c r="C60" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="61" ht="15.35" customHeight="1">
-      <c r="A61" s="12">
-        <v>44410.604163310185</v>
-      </c>
-      <c r="B61" s="9">
-        <v>-48.097</v>
-      </c>
-      <c r="C61" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="62" ht="15.35" customHeight="1">
-      <c r="A62" s="12">
-        <v>44410.614579918984</v>
-      </c>
-      <c r="B62" s="9">
-        <v>-49.305</v>
-      </c>
-      <c r="C62" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="63" ht="15.35" customHeight="1">
-      <c r="A63" s="12">
-        <v>44410.624996527775</v>
-      </c>
-      <c r="B63" s="9">
-        <v>-50.513</v>
-      </c>
-      <c r="C63" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="64" ht="15.35" customHeight="1">
-      <c r="A64" s="12">
-        <v>44410.635413136573</v>
-      </c>
-      <c r="B64" s="9">
-        <v>-51.721</v>
-      </c>
-      <c r="C64" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="65" ht="15.35" customHeight="1">
-      <c r="A65" s="12">
-        <v>44410.645829745372</v>
-      </c>
-      <c r="B65" s="9">
-        <v>-52.929</v>
-      </c>
-      <c r="C65" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="66" ht="15.35" customHeight="1">
-      <c r="A66" s="12">
-        <v>44410.656246354163</v>
-      </c>
-      <c r="B66" s="9">
-        <v>-54.137</v>
-      </c>
-      <c r="C66" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="67" ht="15.35" customHeight="1">
-      <c r="A67" s="12">
-        <v>44410.666662962962</v>
-      </c>
-      <c r="B67" s="9">
-        <v>-55.345</v>
-      </c>
-      <c r="C67" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="68" ht="15.35" customHeight="1">
-      <c r="A68" s="12">
-        <v>44410.677079571760</v>
-      </c>
-      <c r="B68" s="9">
-        <v>-56.553</v>
-      </c>
-      <c r="C68" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="69" ht="15.35" customHeight="1">
-      <c r="A69" s="12">
-        <v>44410.687496180559</v>
-      </c>
-      <c r="B69" s="9">
-        <v>-57.761</v>
-      </c>
-      <c r="C69" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="70" ht="15.35" customHeight="1">
-      <c r="A70" s="12">
-        <v>44410.697912789350</v>
-      </c>
-      <c r="B70" s="9">
-        <v>-58.969</v>
-      </c>
-      <c r="C70" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="71" ht="15.35" customHeight="1">
-      <c r="A71" s="12">
-        <v>44410.708329398149</v>
-      </c>
-      <c r="B71" s="9">
-        <v>-60.177</v>
-      </c>
-      <c r="C71" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="72" ht="15.35" customHeight="1">
-      <c r="A72" s="12">
-        <v>44410.718746006947</v>
-      </c>
-      <c r="B72" s="9">
-        <v>-61.385</v>
-      </c>
-      <c r="C72" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="73" ht="15.35" customHeight="1">
-      <c r="A73" s="12">
-        <v>44410.729162615738</v>
-      </c>
-      <c r="B73" s="9">
-        <v>-62.593</v>
-      </c>
-      <c r="C73" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="74" ht="15.35" customHeight="1">
-      <c r="A74" s="12">
-        <v>44410.739579224537</v>
-      </c>
-      <c r="B74" s="9">
-        <v>-63.801</v>
-      </c>
-      <c r="C74" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="75" ht="15.35" customHeight="1">
-      <c r="A75" s="12">
-        <v>44410.749995833336</v>
-      </c>
-      <c r="B75" s="9">
-        <v>-65.009</v>
-      </c>
-      <c r="C75" s="9">
-        <v>11.5</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
GSYE-703: Adapt CDS parser for different grid_fee variables
</commit_message>
<xml_diff>
--- a/tests/fixtures/community_datasheet.xlsx
+++ b/tests/fixtures/community_datasheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General settings" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
   <si>
     <t xml:space="preserve">start_date</t>
   </si>
@@ -78,7 +78,10 @@
     <t xml:space="preserve">Feed-in Tariff</t>
   </si>
   <si>
-    <t xml:space="preserve">Grid fee</t>
+    <t xml:space="preserve">Grid import fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grid export fee</t>
   </si>
   <si>
     <t xml:space="preserve">Taxes and surcharges</t>
@@ -320,16 +323,16 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1:E3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G1:H4 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="28"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="1" width="10.85"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="1" width="10.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -458,22 +461,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1:E3 A1"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1:H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.35"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.85"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="24.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="5" style="1" width="21.67"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="33.85"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="13" style="1" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="5" style="1" width="21.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="10.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="33.85"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="1" width="10.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -510,64 +513,70 @@
       <c r="K1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="4"/>
+      <c r="L1" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="4"/>
+      <c r="L2" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>64508</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E3" s="4" t="n">
         <v>1</v>
@@ -579,7 +588,7 @@
         <v>0.3</v>
       </c>
       <c r="H3" s="4" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I3" s="4" t="n">
         <v>0.5</v>
@@ -590,24 +599,27 @@
       <c r="K3" s="4" t="n">
         <v>0.5</v>
       </c>
-      <c r="L3" s="4"/>
+      <c r="L3" s="4" t="n">
+        <v>0.5</v>
+      </c>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>57441</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E4" s="4" t="n">
         <v>1</v>
@@ -619,7 +631,7 @@
         <v>0.3</v>
       </c>
       <c r="H4" s="4" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I4" s="4" t="n">
         <v>0.5</v>
@@ -630,11 +642,14 @@
       <c r="K4" s="4" t="n">
         <v>0.5</v>
       </c>
-      <c r="L4" s="4"/>
+      <c r="L4" s="4" t="n">
+        <v>0.5</v>
+      </c>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -658,21 +673,21 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1:E3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G1:H4 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.67"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="1" width="10.85"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="1" width="10.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -680,10 +695,10 @@
     </row>
     <row r="2" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -757,40 +772,40 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1:E3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G1:H4 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.85"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.85"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="10.85"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="10.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="6" t="n">
@@ -800,10 +815,10 @@
     </row>
     <row r="3" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>12</v>
@@ -875,26 +890,26 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1:E3"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="G1:H4 C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="1" width="10.85"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="1" width="10.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -902,10 +917,10 @@
     </row>
     <row r="2" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -913,10 +928,10 @@
     </row>
     <row r="3" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -976,35 +991,35 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1:E3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G1:H4 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="1" width="10.85"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="1" width="10.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
GSYE-804: Add first version of advanced settings parser
</commit_message>
<xml_diff>
--- a/tests/fixtures/community_datasheet.xlsx
+++ b/tests/fixtures/community_datasheet.xlsx
@@ -8,12 +8,13 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="General settings" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Community Members" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Load" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="PV" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Storage" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Profiles" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="General settings" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Advanced settings" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Community Members" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Load" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="PV" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="Storage" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="Profiles" sheetId="7" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
   <si>
     <t xml:space="preserve">start_date</t>
   </si>
@@ -54,10 +55,64 @@
     <t xml:space="preserve">EUR</t>
   </si>
   <si>
-    <t xml:space="preserve">Coefficient type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">constant</t>
+    <t xml:space="preserve">Coefficient algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">str</t>
+  </si>
+  <si>
+    <t xml:space="preserve">static</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grid fees reduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">float</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intracommunity rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operational hours of delay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VAT percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Self consumption scheme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable grid_import_fee_const</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable grid_export_fee_const</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable taxes_surcharges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable marketplace_monthly_fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable assistance_monthly_fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable service_monthly_fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable contracted_power_monthly_fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable contracted_power_cargo_monthly_fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable energy_cargo_fee</t>
   </si>
   <si>
     <t xml:space="preserve">Member list name</t>
@@ -178,14 +233,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="167" formatCode="0.00"/>
-    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd\ hh:mm"/>
+    <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="168" formatCode="0.00"/>
+    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd\ hh:mm"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
@@ -206,6 +262,20 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -270,7 +340,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -291,15 +361,51 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -315,15 +421,121 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G1:H4 A1"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -388,15 +600,9 @@
       <c r="E4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A5" s="0"/>
+      <c r="B5" s="0"/>
+      <c r="C5" s="0"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
@@ -415,34 +621,171 @@
       <c r="E7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4"/>
+      <c r="A8" s="5"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
+    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+    </row>
+    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+    </row>
+    <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+    </row>
+    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+    </row>
+    <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+    </row>
+    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+    </row>
+    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+    </row>
+    <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+    </row>
+    <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+    </row>
+    <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+    </row>
+    <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+    </row>
+    <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+    </row>
+    <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+    </row>
+    <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+    </row>
+    <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+    </row>
+    <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="1">
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4" type="list">
       <formula1>"USD,EUR,JPY,GBP,AUD,CAD,CNY,CHF"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C5" type="list">
-      <formula1>"constant,dynamic"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -457,14 +800,224 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="41.91"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="7" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="7" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C7:C15" type="list">
+      <formula1>"True,False"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1:H4"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -481,40 +1034,40 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
@@ -524,40 +1077,40 @@
     </row>
     <row r="2" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
@@ -567,16 +1120,16 @@
     </row>
     <row r="3" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>64508</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="E3" s="4" t="n">
         <v>1</v>
@@ -610,16 +1163,16 @@
     </row>
     <row r="4" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>32</v>
+        <v>49</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>50</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>57441</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="E4" s="4" t="n">
         <v>1</v>
@@ -665,15 +1218,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G1:H4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -684,10 +1237,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -695,10 +1248,10 @@
     </row>
     <row r="2" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -764,15 +1317,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G1:H4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -785,45 +1338,45 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C2" s="4"/>
-      <c r="D2" s="6" t="n">
+      <c r="D2" s="15" t="n">
         <v>12</v>
       </c>
       <c r="E2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="D3" s="6" t="n">
+      <c r="D3" s="15" t="n">
         <v>32</v>
       </c>
       <c r="E3" s="4" t="n">
@@ -883,15 +1436,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="G1:H4 C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -906,10 +1459,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -917,10 +1470,10 @@
     </row>
     <row r="2" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -928,10 +1481,10 @@
     </row>
     <row r="3" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -983,15 +1536,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G1:H4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1002,205 +1555,205 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="n">
+      <c r="A3" s="16" t="n">
         <v>44410</v>
       </c>
-      <c r="B3" s="6" t="n">
+      <c r="B3" s="15" t="n">
         <v>22.32</v>
       </c>
-      <c r="C3" s="6" t="n">
+      <c r="C3" s="15" t="n">
         <v>11.5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
+      <c r="A4" s="16" t="n">
         <v>44410.0416666667</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="15" t="n">
         <v>20.72</v>
       </c>
-      <c r="C4" s="6" t="n">
+      <c r="C4" s="15" t="n">
         <v>11.5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
+      <c r="A5" s="16" t="n">
         <v>44410.0833333333</v>
       </c>
-      <c r="B5" s="6" t="n">
+      <c r="B5" s="15" t="n">
         <v>18.57</v>
       </c>
-      <c r="C5" s="6" t="n">
+      <c r="C5" s="15" t="n">
         <v>11.5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
+      <c r="A6" s="16" t="n">
         <v>44410.125</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="6" t="n">
+      <c r="C6" s="15" t="n">
         <v>11.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="n">
+      <c r="A7" s="16" t="n">
         <v>44410.1666666667</v>
       </c>
-      <c r="B7" s="6" t="n">
+      <c r="B7" s="15" t="n">
         <v>17.135</v>
       </c>
-      <c r="C7" s="6" t="n">
+      <c r="C7" s="15" t="n">
         <v>11.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="n">
+      <c r="A8" s="16" t="n">
         <v>44410.2083333333</v>
       </c>
-      <c r="B8" s="6" t="n">
+      <c r="B8" s="15" t="n">
         <v>15.927</v>
       </c>
-      <c r="C8" s="6" t="n">
+      <c r="C8" s="15" t="n">
         <v>11.5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="n">
+      <c r="A9" s="16" t="n">
         <v>44410.25</v>
       </c>
-      <c r="B9" s="6" t="n">
+      <c r="B9" s="15" t="n">
         <v>14.719</v>
       </c>
-      <c r="C9" s="6" t="n">
+      <c r="C9" s="15" t="n">
         <v>11.5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="n">
+      <c r="A10" s="16" t="n">
         <v>44410.2916666667</v>
       </c>
-      <c r="B10" s="6" t="n">
+      <c r="B10" s="15" t="n">
         <v>13.511</v>
       </c>
-      <c r="C10" s="6" t="n">
+      <c r="C10" s="15" t="n">
         <v>11.5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="n">
+      <c r="A11" s="16" t="n">
         <v>44410.3333333333</v>
       </c>
-      <c r="B11" s="6" t="n">
+      <c r="B11" s="15" t="n">
         <v>12.303</v>
       </c>
-      <c r="C11" s="6" t="n">
+      <c r="C11" s="15" t="n">
         <v>11.5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="n">
+      <c r="A12" s="16" t="n">
         <v>44410.375</v>
       </c>
-      <c r="B12" s="6" t="n">
+      <c r="B12" s="15" t="n">
         <v>11.095</v>
       </c>
-      <c r="C12" s="6" t="n">
+      <c r="C12" s="15" t="n">
         <v>11.5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="n">
+      <c r="A13" s="16" t="n">
         <v>44410.4166666667</v>
       </c>
-      <c r="B13" s="6" t="n">
+      <c r="B13" s="15" t="n">
         <v>9.887</v>
       </c>
-      <c r="C13" s="6" t="n">
+      <c r="C13" s="15" t="n">
         <v>11.5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="n">
+      <c r="A14" s="16" t="n">
         <v>44410.4583333333</v>
       </c>
-      <c r="B14" s="6" t="n">
+      <c r="B14" s="15" t="n">
         <v>8.679</v>
       </c>
-      <c r="C14" s="6" t="n">
+      <c r="C14" s="15" t="n">
         <v>11.5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="n">
+      <c r="A15" s="16" t="n">
         <v>44410.5</v>
       </c>
-      <c r="B15" s="6" t="n">
+      <c r="B15" s="15" t="n">
         <v>7.471</v>
       </c>
-      <c r="C15" s="6" t="n">
+      <c r="C15" s="15" t="n">
         <v>11.5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="n">
+      <c r="A16" s="16" t="n">
         <v>44410.5416666667</v>
       </c>
-      <c r="B16" s="6" t="n">
+      <c r="B16" s="15" t="n">
         <v>6.263</v>
       </c>
-      <c r="C16" s="6" t="n">
+      <c r="C16" s="15" t="n">
         <v>11.5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="n">
+      <c r="A17" s="16" t="n">
         <v>44410.5833333333</v>
       </c>
-      <c r="B17" s="6" t="n">
+      <c r="B17" s="15" t="n">
         <v>5.055</v>
       </c>
-      <c r="C17" s="6" t="n">
+      <c r="C17" s="15" t="n">
         <v>11.5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="n">
+      <c r="A18" s="16" t="n">
         <v>44410.625</v>
       </c>
-      <c r="B18" s="6" t="n">
+      <c r="B18" s="15" t="n">
         <v>3.847</v>
       </c>
-      <c r="C18" s="6" t="n">
+      <c r="C18" s="15" t="n">
         <v>11.5</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="n">
+      <c r="A19" s="16" t="n">
         <v>44410.6666666667</v>
       </c>
-      <c r="B19" s="6" t="n">
+      <c r="B19" s="15" t="n">
         <v>2.639</v>
       </c>
       <c r="C19" s="4"/>

</xml_diff>

<commit_message>
GSYE-807: Make CDS advanced settings naming more explixit
</commit_message>
<xml_diff>
--- a/tests/fixtures/community_datasheet.xlsx
+++ b/tests/fixtures/community_datasheet.xlsx
@@ -85,34 +85,34 @@
     <t xml:space="preserve">int</t>
   </si>
   <si>
-    <t xml:space="preserve">Enable grid_import_fee_const</t>
+    <t xml:space="preserve">Enable grid import fee</t>
   </si>
   <si>
     <t xml:space="preserve">bool</t>
   </si>
   <si>
-    <t xml:space="preserve">Enable grid_export_fee_const</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enable taxes_surcharges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enable marketplace_monthly_fee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enable assistance_monthly_fee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enable service_monthly_fee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enable contracted_power_monthly_fee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enable contracted_power_cargo_monthly_fee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enable energy_cargo_fee</t>
+    <t xml:space="preserve">Enable grid export fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable taxes surcharges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable marketplace monthly fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable assistance monthly fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable service monthly fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable contracted power monthly fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable contracted power cargo monthly fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable energy cargo fee</t>
   </si>
   <si>
     <t xml:space="preserve">Member list name</t>
@@ -799,7 +799,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>